<commit_message>
removed key, added more structure
</commit_message>
<xml_diff>
--- a/list.xlsx
+++ b/list.xlsx
@@ -1,13 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
+  <bookViews>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="1"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Intersections" sheetId="1" r:id="rId3"/>
-    <sheet state="visible" name="Buildings" sheetId="2" r:id="rId4"/>
+    <sheet name="Intersections" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Buildings" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
@@ -71,31 +75,71 @@
     <t>30.290875, -97.738999</t>
   </si>
   <si>
-    <t>Duren</t>
-  </si>
-  <si>
-    <t>Residence Hall</t>
+    <t>Duren Residence Hall</t>
+  </si>
+  <si>
+    <t>30.291554, -97.740661</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
-    <font>
-      <sz val="10.0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
+  </numFmts>
+  <fonts count="9">
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-    </font>
-    <font/>
-    <font>
-      <sz val="9.0"/>
-    </font>
-    <font>
-      <sz val="10.0"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Cambria"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -103,73 +147,109 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
+  <cellXfs count="7">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="0"/>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/worksheetdrawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/worksheetdrawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A73" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A97" activeCellId="0" sqref="A97"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="22.0"/>
-    <col customWidth="1" min="2" max="2" width="20.43"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.4285714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="14.4285714285714"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -180,7 +260,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -189,7 +269,7 @@
       </c>
       <c r="C2" s="3"/>
     </row>
-    <row r="3">
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -198,7 +278,7 @@
       </c>
       <c r="C3" s="4"/>
     </row>
-    <row r="4">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -207,7 +287,7 @@
       </c>
       <c r="C4" s="4"/>
     </row>
-    <row r="5">
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -215,7 +295,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -223,7 +303,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -231,7 +311,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -239,7 +319,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
@@ -248,32 +328,49 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A2:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="14.4285714285714"/>
+  </cols>
   <sheetData>
-    <row r="2">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="2">
-        <v>30.291554</v>
-      </c>
-      <c r="D2" s="5">
-        <v>-97.740661</v>
-      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="6"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>